<commit_message>
automating working osim creation
</commit_message>
<xml_diff>
--- a/FMC_OpenSim/models/fmc_hand_model/hand_joints.xlsx
+++ b/FMC_OpenSim/models/fmc_hand_model/hand_joints.xlsx
@@ -1138,12 +1138,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>/bodyset/capitate</t>
+          <t>/bodyset/trapezoid</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>'0.014685 -0.037620000000000001 0.005032</t>
+          <t>'0 0 0</t>
         </is>
       </c>
     </row>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>'0 0 0</t>
+          <t>'-0.0047000000000000002 0.033500000000000002 -0.0089999999999999993</t>
         </is>
       </c>
     </row>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>'-0.012045999999999999 -0.040518999999999999 0.0035130000000000001</t>
+          <t>'0 0 0</t>
         </is>
       </c>
     </row>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>'0 0 0</t>
+          <t>'0.012999999999999999 0.040000000000000001 -0.0050000000000000001</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>'-0.021895999999999999 -0.034682999999999999 -0.0042180000000000004</t>
+          <t>'0 0 0</t>
         </is>
       </c>
     </row>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>'0 0 0</t>
+          <t>'0.02 0.035999999999999997 0.0050000000000000001</t>
         </is>
       </c>
     </row>

</xml_diff>